<commit_message>
added pcb board to the BOM
</commit_message>
<xml_diff>
--- a/Parts/BOM_Arduino_Spot_Welder.xlsx
+++ b/Parts/BOM_Arduino_Spot_Welder.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Quantity</t>
   </si>
@@ -212,6 +212,15 @@
   </si>
   <si>
     <t>Aliexpress.com</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>from pcb manufacturer</t>
+  </si>
+  <si>
+    <t>pcbway.com  (you get 10 pcbs for this price)</t>
   </si>
 </sst>
 </file>
@@ -269,7 +278,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -462,12 +471,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -521,28 +545,35 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -848,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H30"/>
+  <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,10 +896,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="25" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1148,7 +1179,7 @@
         <v>46</v>
       </c>
       <c r="F18" s="17"/>
-      <c r="G18" s="26">
+      <c r="G18" s="23">
         <v>0.06</v>
       </c>
       <c r="H18" s="18" t="s">
@@ -1161,124 +1192,142 @@
     <row r="20" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="22" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="21" spans="3:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="21">
-        <v>1</v>
-      </c>
-      <c r="D21" s="21" t="s">
+      <c r="C21" s="26">
+        <v>1</v>
+      </c>
+      <c r="D21" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="4">
+      <c r="E21" s="26"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="31">
         <v>1.7</v>
       </c>
-      <c r="H21" s="22" t="s">
+      <c r="H21" s="32" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="22" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="2">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="C22" s="30">
+        <v>1</v>
+      </c>
+      <c r="D22" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="25">
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="33">
         <v>2</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="27" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="23" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="2">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="C23" s="30">
+        <v>1</v>
+      </c>
+      <c r="D23" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="25">
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="33">
         <v>0</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="27" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="24" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="2">
-        <v>1</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="C24" s="30">
+        <v>1</v>
+      </c>
+      <c r="D24" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="25">
-        <v>1</v>
-      </c>
-      <c r="H24" s="3" t="s">
+      <c r="F24" s="30"/>
+      <c r="G24" s="33">
+        <v>1</v>
+      </c>
+      <c r="H24" s="27" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="25" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="2">
+      <c r="C25" s="30">
         <v>3</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2">
+      <c r="E25" s="30"/>
+      <c r="F25" s="30">
         <v>0.6</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="31">
         <v>1.8</v>
       </c>
-      <c r="H25" s="22" t="s">
+      <c r="H25" s="32" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="26" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="21">
-        <v>1</v>
-      </c>
-      <c r="D26" s="21" t="s">
+      <c r="C26" s="26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="27">
+      <c r="F26" s="27"/>
+      <c r="G26" s="28">
         <v>1.95</v>
       </c>
-      <c r="H26" s="28" t="s">
+      <c r="H26" s="29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="E28" s="23" t="s">
+    <row r="27" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="26">
+        <v>1</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="27"/>
+      <c r="G27" s="28">
+        <v>20</v>
+      </c>
+      <c r="H27" s="29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E29" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="G28" s="29">
-        <f>SUM(G5:G27)</f>
-        <v>27.443999999999996</v>
-      </c>
-    </row>
-    <row r="29" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="G29" s="24">
+        <f>SUM(G5:G28)</f>
+        <v>47.443999999999996</v>
+      </c>
+    </row>
     <row r="30" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H5" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Reichelt Part List
</commit_message>
<xml_diff>
--- a/Parts/BOM_Arduino_Spot_Welder.xlsx
+++ b/Parts/BOM_Arduino_Spot_Welder.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -881,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="9" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>15</v>
@@ -1012,9 +1012,11 @@
       <c r="E9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="4">
+        <v>0.26</v>
+      </c>
       <c r="G9" s="4">
-        <v>0.26</v>
+        <v>0.78</v>
       </c>
       <c r="H9" s="14" t="s">
         <v>17</v>
@@ -1323,7 +1325,7 @@
       </c>
       <c r="G29" s="24">
         <f>SUM(G5:G28)</f>
-        <v>47.583999999999996</v>
+        <v>48.103999999999999</v>
       </c>
     </row>
     <row r="30" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>